<commit_message>
corrected pf results for wp2.5; adjusted pf_shortcircuit_analysis.py
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_isolated.xlsx
+++ b/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_isolated.xlsx
@@ -716,49 +716,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.54545480308452</v>
+        <v>4.545454803106412</v>
       </c>
       <c r="D2">
-        <v>4.54545480308452</v>
+        <v>4.545454803106412</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>288.6751509565138</v>
+        <v>288.6751509579041</v>
       </c>
       <c r="G2">
-        <v>288.6751509565138</v>
+        <v>288.6751509579041</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.9526279647803683</v>
+        <v>0.9526279647803685</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.9526279647833883</v>
+        <v>0.9526279647833882</v>
       </c>
       <c r="Q2">
-        <v>-8.693883187637584E-11</v>
+        <v>-8.693997994959665E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -808,22 +808,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.952627964667196</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>1.45740960157308E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999998456</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -867,22 +867,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.9526279646404244</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.9526279649233318</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>1.564854331620535E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.9999999984264</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -926,22 +926,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.9526279646315008</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>2.037891952334428E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -985,22 +985,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.9526279646315009</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>2.037888002295718E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
   </sheetData>
@@ -1083,55 +1083,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.734156921382979</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="D2">
-        <v>3.734156921382979</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>237.1508154132444</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="G2">
-        <v>237.1508154132444</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>1.020226441411962</v>
+        <v>1.020226441408047</v>
       </c>
       <c r="O2">
-        <v>0.2400406982762188</v>
+        <v>0.240040698275847</v>
       </c>
       <c r="P2">
-        <v>0.8960735769109617</v>
+        <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884843866</v>
+        <v>5.766209884997124</v>
       </c>
       <c r="R2">
-        <v>-121.3466079985248</v>
+        <v>-121.3466079962484</v>
       </c>
       <c r="S2">
-        <v>173.4315681773925</v>
+        <v>173.4315681772755</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1175,22 +1175,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>1.02022644131502</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0.2400406981630188</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.8960735770061724</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>5.766209884977172</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079609366</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>173.4315681785684</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1234,22 +1234,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0.2400406981651692</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.8960735770323204</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>5.766209886018052</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079469511</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>173.4315681777209</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1293,22 +1293,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>5.766209886365012</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079422893</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1352,22 +1352,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>5.76620988636501</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079422893</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
   </sheetData>
@@ -1450,55 +1450,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.734156921382979</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="D2">
-        <v>3.734156921382979</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>237.1508154132444</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="G2">
-        <v>237.1508154132444</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>1.020226441411962</v>
+        <v>1.020226441408047</v>
       </c>
       <c r="O2">
-        <v>0.2400406982762188</v>
+        <v>0.240040698275847</v>
       </c>
       <c r="P2">
-        <v>0.8960735769109617</v>
+        <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884843866</v>
+        <v>5.766209884997124</v>
       </c>
       <c r="R2">
-        <v>-121.3466079985248</v>
+        <v>-121.3466079962484</v>
       </c>
       <c r="S2">
-        <v>173.4315681773925</v>
+        <v>173.4315681772755</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1542,22 +1542,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>1.02022644131502</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0.2400406981630188</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.8960735770061724</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>5.766209884977172</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079609366</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>173.4315681785684</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1601,22 +1601,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0.2400406981651692</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.8960735770323204</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>5.766209886018052</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079469511</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>173.4315681777209</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1660,22 +1660,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>5.766209886365012</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079422893</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1719,22 +1719,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>5.76620988636501</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-121.3466079422893</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
   </sheetData>
@@ -1817,55 +1817,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.63636376373438</v>
+        <v>3.636363763754282</v>
       </c>
       <c r="D2">
-        <v>3.63636376373438</v>
+        <v>3.636363763754282</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>230.940115764979</v>
+        <v>230.9401157662429</v>
       </c>
       <c r="G2">
-        <v>230.940115764979</v>
+        <v>230.9401157662429</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.8660254037845058</v>
+        <v>0.8660254037845059</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.8660254037849897</v>
+        <v>0.8660254037849899</v>
       </c>
       <c r="Q2">
-        <v>1.720091434129778E-10</v>
+        <v>1.719980025483599E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999998193</v>
+        <v>179.9999999998194</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1909,22 +1909,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.8660254036789682</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.8660254038905275</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>4.107191710696312E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999995807</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1968,22 +1968,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.866025403654631</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.8660254039148652</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>3.135417159618479E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.999999996856</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2027,22 +2027,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.8660254036465186</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>4.04364590770589E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999959477</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2086,22 +2086,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.8660254036465187</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>4.043652863043647E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999959477</v>
       </c>
     </row>
   </sheetData>
@@ -2184,55 +2184,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.63636376373438</v>
+        <v>3.636363763754282</v>
       </c>
       <c r="D2">
-        <v>3.63636376373438</v>
+        <v>3.636363763754282</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>230.940115764979</v>
+        <v>230.9401157662429</v>
       </c>
       <c r="G2">
-        <v>230.940115764979</v>
+        <v>230.9401157662429</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.8660254037845058</v>
+        <v>0.8660254037845059</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.8660254037849897</v>
+        <v>0.8660254037849899</v>
       </c>
       <c r="Q2">
-        <v>1.720091434129778E-10</v>
+        <v>1.719980025483599E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999998193</v>
+        <v>179.9999999998194</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2276,22 +2276,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.8660254036789682</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.8660254038905275</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>4.107191710696312E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999995807</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2335,22 +2335,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.866025403654631</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.8660254039148652</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>3.135417159618479E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.999999996856</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2394,22 +2394,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.8660254036465186</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>4.04364590770589E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999959477</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2453,22 +2453,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.8660254036465187</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>4.043652863043647E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999959477</v>
       </c>
     </row>
   </sheetData>
@@ -2551,55 +2551,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.055365721225704</v>
+        <v>3.055365721222171</v>
       </c>
       <c r="D2">
-        <v>3.055365721225704</v>
+        <v>3.055365721222171</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>194.0417843784657</v>
+        <v>194.0417843782413</v>
       </c>
       <c r="G2">
-        <v>194.0417843784657</v>
+        <v>194.0417843782413</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.9220324944375794</v>
+        <v>0.9220324944339026</v>
       </c>
       <c r="O2">
-        <v>0.1964063473245135</v>
+        <v>0.1964063473242862</v>
       </c>
       <c r="P2">
-        <v>0.8180121061777103</v>
+        <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
-        <v>5.173976903950488</v>
+        <v>5.173976904115779</v>
       </c>
       <c r="R2">
-        <v>-122.1449202988061</v>
+        <v>-122.1449202961592</v>
       </c>
       <c r="S2">
-        <v>174.1659345854433</v>
+        <v>174.1659345853096</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2643,22 +2643,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.9220324943451753</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.1964063472166732</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.8180121062689185</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>5.173976904114584</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202549971</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>174.1659345864976</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2702,22 +2702,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.9220324943235488</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.1964063472443386</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.8180121062966166</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>5.173976906219912</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202329787</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>174.1659345844575</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2761,22 +2761,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.92203249431634</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.1964063472535604</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>5.173976906921688</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202256392</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>174.1659345837774</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2820,22 +2820,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.92203249431634</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.1964063472535604</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.8180121063058494</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>5.173976906921695</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202256392</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>174.1659345837774</v>
       </c>
     </row>
   </sheetData>
@@ -2918,55 +2918,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.055365721225704</v>
+        <v>3.055365721222171</v>
       </c>
       <c r="D2">
-        <v>3.055365721225704</v>
+        <v>3.055365721222171</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>194.0417843784657</v>
+        <v>194.0417843782413</v>
       </c>
       <c r="G2">
-        <v>194.0417843784657</v>
+        <v>194.0417843782413</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.9220324944375794</v>
+        <v>0.9220324944339026</v>
       </c>
       <c r="O2">
-        <v>0.1964063473245135</v>
+        <v>0.1964063473242862</v>
       </c>
       <c r="P2">
-        <v>0.8180121061777103</v>
+        <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
-        <v>5.173976903950488</v>
+        <v>5.173976904115779</v>
       </c>
       <c r="R2">
-        <v>-122.1449202988061</v>
+        <v>-122.1449202961592</v>
       </c>
       <c r="S2">
-        <v>174.1659345854433</v>
+        <v>174.1659345853096</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3010,22 +3010,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.9220324943451753</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.1964063472166732</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.8180121062689185</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>5.173976904114584</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202549971</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>174.1659345864976</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3069,22 +3069,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.9220324943235488</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.1964063472443386</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.8180121062966166</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>5.173976906219912</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202329787</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>174.1659345844575</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3128,22 +3128,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.92203249431634</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.1964063472535604</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>5.173976906921688</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202256392</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>174.1659345837774</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3187,22 +3187,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.92203249431634</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.1964063472535604</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.8180121063058494</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>5.173976906921695</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-122.1449202256392</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>174.1659345837774</v>
       </c>
     </row>
   </sheetData>
@@ -3282,7 +3282,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5.248639108456902</v>
+        <v>5.248639108526414</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>333.3333522361469</v>
+        <v>333.3333522405615</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3300,40 +3300,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.324394473472893</v>
+        <v>1.324394477419441</v>
       </c>
       <c r="I2">
-        <v>13.24394453576718</v>
+        <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394472531988</v>
+        <v>1.324394473163435</v>
       </c>
       <c r="K2">
-        <v>13.24394453576793</v>
+        <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.324394473472896</v>
+        <v>1.32439447410434</v>
       </c>
       <c r="M2">
-        <v>13.24394453576718</v>
+        <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6350853099230456</v>
+        <v>0.6350853098740156</v>
       </c>
       <c r="O2">
         <v>1.100000023884844</v>
       </c>
       <c r="P2">
-        <v>0.6350853098972609</v>
+        <v>0.6350853099409384</v>
       </c>
       <c r="Q2">
-        <v>59.99999999884959</v>
+        <v>59.99999999685337</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999636</v>
+        <v>-89.99999999999633</v>
       </c>
       <c r="S2">
-        <v>120.0000000024862</v>
+        <v>119.9999999996535</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3377,22 +3377,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6350853099894118</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6350853098300098</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>60.00000000239918</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>120.0000000058974</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3436,22 +3436,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6350853100298056</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6350853098168613</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>60.00000000166495</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>120.0000000094205</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3495,22 +3495,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.6350853100432702</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6350853098124783</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>60.0000000014202</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>120.0000000105949</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3554,22 +3554,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.6350853100432702</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6350853098124781</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>60.00000000142021</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>120.0000000105949</v>
       </c>
     </row>
   </sheetData>
@@ -3649,7 +3649,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5.248639108456902</v>
+        <v>5.248639108526414</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>333.3333522361469</v>
+        <v>333.3333522405615</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3667,40 +3667,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.324394473472893</v>
+        <v>1.324394477419441</v>
       </c>
       <c r="I2">
-        <v>13.24394453576718</v>
+        <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394472531988</v>
+        <v>1.324394473163435</v>
       </c>
       <c r="K2">
-        <v>13.24394453576793</v>
+        <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.324394473472896</v>
+        <v>1.32439447410434</v>
       </c>
       <c r="M2">
-        <v>13.24394453576718</v>
+        <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6350853099230456</v>
+        <v>0.6350853098740156</v>
       </c>
       <c r="O2">
         <v>1.100000023884844</v>
       </c>
       <c r="P2">
-        <v>0.6350853098972609</v>
+        <v>0.6350853099409384</v>
       </c>
       <c r="Q2">
-        <v>59.99999999884959</v>
+        <v>59.99999999685337</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999636</v>
+        <v>-89.99999999999633</v>
       </c>
       <c r="S2">
-        <v>120.0000000024862</v>
+        <v>119.9999999996535</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3744,22 +3744,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6350853099894118</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6350853098300098</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>60.00000000239918</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>120.0000000058974</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3803,22 +3803,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6350853100298056</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6350853098168613</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>60.00000000166495</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>120.0000000094205</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3862,22 +3862,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.6350853100432702</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6350853098124783</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>60.0000000014202</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>120.0000000105949</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3921,22 +3921,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.6350853100432702</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6350853098124781</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>60.00000000142021</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>120.0000000105949</v>
       </c>
     </row>
   </sheetData>
@@ -4016,7 +4016,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.617960382517467</v>
+        <v>3.617960382473003</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4025,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>229.7713440840247</v>
+        <v>229.7713440812009</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -4034,40 +4034,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.324394473472893</v>
+        <v>1.324394477419441</v>
       </c>
       <c r="I2">
-        <v>13.24394453576718</v>
+        <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394472531988</v>
+        <v>1.324394473163435</v>
       </c>
       <c r="K2">
-        <v>13.24394453576793</v>
+        <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.324394473472896</v>
+        <v>1.32439447410434</v>
       </c>
       <c r="M2">
-        <v>13.24394453576718</v>
+        <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6918398877296293</v>
+        <v>0.6918398877278027</v>
       </c>
       <c r="O2">
         <v>1.100000023874158</v>
       </c>
       <c r="P2">
-        <v>0.837842757876562</v>
+        <v>0.8378427578966809</v>
       </c>
       <c r="Q2">
-        <v>40.4095179577123</v>
+        <v>40.40951795604943</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999653</v>
+        <v>-89.99999999999652</v>
       </c>
       <c r="S2">
-        <v>128.9574716957084</v>
+        <v>128.9574716956184</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4111,22 +4111,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6918398877714428</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.83784275781675</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>40.40951796258043</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>128.9574716984651</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4170,22 +4170,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6918398877978506</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.8378427578056247</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>40.40951796344665</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>128.9574717002523</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4229,22 +4229,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.6918398878066531</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>40.40951796373539</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>128.9574717008481</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -4288,22 +4288,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.691839887806653</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>40.4095179637354</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>128.9574717008481</v>
       </c>
     </row>
   </sheetData>
@@ -4534,7 +4534,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.617960382517467</v>
+        <v>3.617960382473003</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4543,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>229.7713440840247</v>
+        <v>229.7713440812009</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -4552,40 +4552,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.324394473472893</v>
+        <v>1.324394477419441</v>
       </c>
       <c r="I2">
-        <v>13.24394453576718</v>
+        <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394472531988</v>
+        <v>1.324394473163435</v>
       </c>
       <c r="K2">
-        <v>13.24394453576793</v>
+        <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.324394473472896</v>
+        <v>1.32439447410434</v>
       </c>
       <c r="M2">
-        <v>13.24394453576718</v>
+        <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6918398877296293</v>
+        <v>0.6918398877278027</v>
       </c>
       <c r="O2">
         <v>1.100000023874158</v>
       </c>
       <c r="P2">
-        <v>0.837842757876562</v>
+        <v>0.8378427578966809</v>
       </c>
       <c r="Q2">
-        <v>40.4095179577123</v>
+        <v>40.40951795604943</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999653</v>
+        <v>-89.99999999999652</v>
       </c>
       <c r="S2">
-        <v>128.9574716957084</v>
+        <v>128.9574716956184</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4629,22 +4629,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6918398877714428</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.83784275781675</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>40.40951796258043</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>128.9574716984651</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4688,22 +4688,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6918398877978506</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.8378427578056247</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>40.40951796344665</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>128.9574717002523</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4747,22 +4747,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.6918398878066531</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>40.40951796373539</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>128.9574717008481</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -4806,22 +4806,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.691839887806653</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>1.100000023874166</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>40.4095179637354</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>128.9574717008481</v>
       </c>
     </row>
   </sheetData>
@@ -4901,7 +4901,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>4.198911195729429</v>
+        <v>4.198911195792623</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4910,7 +4910,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>266.6666760073492</v>
+        <v>266.6666760113625</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -4919,40 +4919,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993719880022</v>
+        <v>1.504993724976286</v>
       </c>
       <c r="I2">
-        <v>15.04993697245777</v>
+        <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993721833392</v>
+        <v>1.504993722648792</v>
       </c>
       <c r="K2">
-        <v>15.04993697245861</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993719880027</v>
+        <v>1.50499372069543</v>
       </c>
       <c r="M2">
-        <v>15.04993697245777</v>
+        <v>15.04993697229304</v>
       </c>
       <c r="N2">
-        <v>0.5773502691662145</v>
+        <v>0.5773502691155638</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962953</v>
+        <v>0.9999999999962959</v>
       </c>
       <c r="P2">
-        <v>0.5773502692090567</v>
+        <v>0.5773502692541784</v>
       </c>
       <c r="Q2">
-        <v>59.99999999874468</v>
+        <v>59.99999999647623</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S2">
-        <v>119.9999999987934</v>
+        <v>119.9999999955744</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4996,22 +4996,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.577350269223176</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.9999999999962963</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.5773502691507328</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>60.00000000216502</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>120.0000000019794</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5055,22 +5055,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.5773502692712909</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.5773502691501733</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>59.99999999947238</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>120.0000000074609</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5114,22 +5114,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.5773502692873292</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>120.000000009288</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -5173,22 +5173,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5773502692873292</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.5773502691499864</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999586</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>120.000000009288</v>
       </c>
     </row>
   </sheetData>
@@ -5268,7 +5268,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>4.198911195729429</v>
+        <v>4.198911195792623</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5277,7 +5277,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>266.6666760073492</v>
+        <v>266.6666760113625</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5286,40 +5286,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993719880022</v>
+        <v>1.504993724976286</v>
       </c>
       <c r="I2">
-        <v>15.04993697245777</v>
+        <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993721833392</v>
+        <v>1.504993722648792</v>
       </c>
       <c r="K2">
-        <v>15.04993697245861</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993719880027</v>
+        <v>1.50499372069543</v>
       </c>
       <c r="M2">
-        <v>15.04993697245777</v>
+        <v>15.04993697229304</v>
       </c>
       <c r="N2">
-        <v>0.5773502691662145</v>
+        <v>0.5773502691155638</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962953</v>
+        <v>0.9999999999962959</v>
       </c>
       <c r="P2">
-        <v>0.5773502692090567</v>
+        <v>0.5773502692541784</v>
       </c>
       <c r="Q2">
-        <v>59.99999999874468</v>
+        <v>59.99999999647623</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S2">
-        <v>119.9999999987934</v>
+        <v>119.9999999955744</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5363,22 +5363,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.577350269223176</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.9999999999962963</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.5773502691507328</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>60.00000000216502</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>120.0000000019794</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5422,22 +5422,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.5773502692712909</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.5773502691501733</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>59.99999999947238</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>120.0000000074609</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5481,22 +5481,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.5773502692873292</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999585</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>120.000000009288</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -5540,22 +5540,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5773502692873292</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.9999999999962964</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.5773502691499864</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999586</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>120.000000009288</v>
       </c>
     </row>
   </sheetData>
@@ -5635,7 +5635,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.012913138794057</v>
+        <v>3.012913138756735</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5644,7 +5644,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>191.345683290048</v>
+        <v>191.3456832876778</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5653,40 +5653,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993719880022</v>
+        <v>1.504993724976286</v>
       </c>
       <c r="I2">
-        <v>15.04993697245777</v>
+        <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993721833392</v>
+        <v>1.504993722648792</v>
       </c>
       <c r="K2">
-        <v>15.04993697245861</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993719880027</v>
+        <v>1.50499372069543</v>
       </c>
       <c r="M2">
-        <v>15.04993697245777</v>
+        <v>15.04993697229304</v>
       </c>
       <c r="N2">
-        <v>0.6184267549991423</v>
+        <v>0.6184267549947473</v>
       </c>
       <c r="O2">
-        <v>0.9999999999908644</v>
+        <v>0.9999999999908646</v>
       </c>
       <c r="P2">
-        <v>0.7472997527121603</v>
+        <v>0.7472997527351809</v>
       </c>
       <c r="Q2">
-        <v>41.77463363330364</v>
+        <v>41.77463363119259</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999652</v>
+        <v>-89.99999999999653</v>
       </c>
       <c r="S2">
-        <v>128.1091583199064</v>
+        <v>128.1091583196818</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5730,22 +5730,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.6184267550404212</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.7472997526577982</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>41.77463363810638</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>128.1091583228107</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5789,22 +5789,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.6184267550800501</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.7472997526545258</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>41.77463363817497</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>128.1091583258392</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5848,22 +5848,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.6184267550932597</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.7472997526534348</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>128.1091583268488</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -5907,22 +5907,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.6184267550932597</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.7472997526534348</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>128.1091583268488</v>
       </c>
     </row>
   </sheetData>
@@ -6002,7 +6002,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.012913138794057</v>
+        <v>3.012913138756735</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -6011,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>191.345683290048</v>
+        <v>191.3456832876778</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -6020,40 +6020,40 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993719880022</v>
+        <v>1.504993724976286</v>
       </c>
       <c r="I2">
-        <v>15.04993697245777</v>
+        <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993721833392</v>
+        <v>1.504993722648792</v>
       </c>
       <c r="K2">
-        <v>15.04993697245861</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993719880027</v>
+        <v>1.50499372069543</v>
       </c>
       <c r="M2">
-        <v>15.04993697245777</v>
+        <v>15.04993697229304</v>
       </c>
       <c r="N2">
-        <v>0.6184267549991423</v>
+        <v>0.6184267549947473</v>
       </c>
       <c r="O2">
-        <v>0.9999999999908644</v>
+        <v>0.9999999999908646</v>
       </c>
       <c r="P2">
-        <v>0.7472997527121603</v>
+        <v>0.7472997527351809</v>
       </c>
       <c r="Q2">
-        <v>41.77463363330364</v>
+        <v>41.77463363119259</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999652</v>
+        <v>-89.99999999999653</v>
       </c>
       <c r="S2">
-        <v>128.1091583199064</v>
+        <v>128.1091583196818</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6097,22 +6097,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.6184267550404212</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.7472997526577982</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>41.77463363810638</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>128.1091583228107</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6156,22 +6156,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.6184267550800501</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.7472997526545258</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>41.77463363817497</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>128.1091583258392</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6215,22 +6215,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.6184267550932597</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.7472997526534348</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>128.1091583268488</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -6274,22 +6274,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.6184267550932597</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.9999999999908713</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.7472997526534348</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-89.99999999999616</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>128.1091583268488</v>
       </c>
     </row>
   </sheetData>
@@ -6372,55 +6372,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.248639108306365</v>
+        <v>5.24863910873685</v>
       </c>
       <c r="D2">
-        <v>5.24863910830651</v>
+        <v>5.248639107970815</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>333.3333522265865</v>
+        <v>333.333352253926</v>
       </c>
       <c r="G2">
-        <v>333.3333522265958</v>
+        <v>333.3333522052762</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.6350853098400608</v>
+        <v>0.6350853098347083</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098560606</v>
+        <v>0.6350853098507082</v>
       </c>
       <c r="Q2">
-        <v>-4.857026428804568E-11</v>
+        <v>-4.877410066046854E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-179.9999999991136</v>
+        <v>179.999999996043</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6464,22 +6464,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6350853097237744</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6350853099661091</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>1.36724273386936E-09</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>-179.9999999983958</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6523,22 +6523,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6350853097106257</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6350853100065029</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>4.890354000285714E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>-179.9999999991301</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6582,22 +6582,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.635085309706243</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6350853100199675</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>6.064709293135375E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>-179.9999999993748</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -6641,22 +6641,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.6350853097062428</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6350853100199674</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>6.06471273289669E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>-179.9999999993748</v>
       </c>
     </row>
   </sheetData>
@@ -6739,55 +6739,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.248639108306365</v>
+        <v>5.24863910873685</v>
       </c>
       <c r="D2">
-        <v>5.24863910830651</v>
+        <v>5.248639107970815</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>333.3333522265865</v>
+        <v>333.333352253926</v>
       </c>
       <c r="G2">
-        <v>333.3333522265958</v>
+        <v>333.3333522052762</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.6350853098400608</v>
+        <v>0.6350853098347083</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098560606</v>
+        <v>0.6350853098507082</v>
       </c>
       <c r="Q2">
-        <v>-4.857026428804568E-11</v>
+        <v>-4.877410066046854E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-179.9999999991136</v>
+        <v>179.999999996043</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6831,22 +6831,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.6350853097237744</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6350853099661091</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>1.36724273386936E-09</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>-179.9999999983958</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6890,22 +6890,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.6350853097106257</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6350853100065029</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>4.890354000285714E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>-179.9999999991301</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6949,22 +6949,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.635085309706243</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6350853100199675</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>6.064709293135375E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>-179.9999999993748</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -7008,22 +7008,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.6350853097062428</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6350853100199674</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>6.06471273289669E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>-179.9999999993748</v>
       </c>
     </row>
   </sheetData>
@@ -7106,55 +7106,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.617960382442754</v>
+        <v>3.617960382593722</v>
       </c>
       <c r="D2">
-        <v>3.617960382442808</v>
+        <v>3.617960382231206</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>229.7713440792798</v>
+        <v>229.7713440888676</v>
       </c>
       <c r="G2">
-        <v>229.7713440792833</v>
+        <v>229.7713440658447</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.8378427578245271</v>
+        <v>0.8378427578256962</v>
       </c>
       <c r="O2">
-        <v>0.4028253111916907</v>
+        <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398876778908</v>
+        <v>0.6918398877011798</v>
       </c>
       <c r="Q2">
-        <v>8.957471694767792</v>
+        <v>8.957471693504784</v>
       </c>
       <c r="R2">
-        <v>-115.8807585983535</v>
+        <v>-115.8807585964592</v>
       </c>
       <c r="S2">
-        <v>160.4095179582256</v>
+        <v>160.4095179569557</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7198,22 +7198,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.8378427577457516</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0.4028253110952157</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6918398877448085</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>8.957471696351657</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-115.8807585788046</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>160.4095179634873</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7257,22 +7257,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.8378427577346264</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0.4028253110970201</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6918398877712161</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>8.957471698138823</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-115.8807585718119</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>160.4095179643536</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -7316,22 +7316,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0.4028253110976215</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>8.957471698734539</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-115.880758569481</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>160.4095179646423</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -7375,22 +7375,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0.4028253110976215</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>8.957471698734546</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-115.880758569481</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>160.4095179646423</v>
       </c>
     </row>
   </sheetData>
@@ -7473,55 +7473,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.617960382442754</v>
+        <v>3.617960382593722</v>
       </c>
       <c r="D2">
-        <v>3.617960382442808</v>
+        <v>3.617960382231206</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>229.7713440792798</v>
+        <v>229.7713440888676</v>
       </c>
       <c r="G2">
-        <v>229.7713440792833</v>
+        <v>229.7713440658447</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.8378427578245271</v>
+        <v>0.8378427578256962</v>
       </c>
       <c r="O2">
-        <v>0.4028253111916907</v>
+        <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398876778908</v>
+        <v>0.6918398877011798</v>
       </c>
       <c r="Q2">
-        <v>8.957471694767792</v>
+        <v>8.957471693504784</v>
       </c>
       <c r="R2">
-        <v>-115.8807585983535</v>
+        <v>-115.8807585964592</v>
       </c>
       <c r="S2">
-        <v>160.4095179582256</v>
+        <v>160.4095179569557</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7565,22 +7565,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.8378427577457516</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0.4028253110952157</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.6918398877448085</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>8.957471696351657</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-115.8807585788046</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>160.4095179634873</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7624,22 +7624,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.8378427577346264</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0.4028253110970201</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.6918398877712161</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>8.957471698138823</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-115.8807585718119</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>160.4095179643536</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -7683,22 +7683,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0.4028253110976215</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>8.957471698734539</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-115.880758569481</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>160.4095179646423</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -7742,22 +7742,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0.4028253110976215</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>8.957471698734546</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-115.880758569481</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>160.4095179646423</v>
       </c>
     </row>
   </sheetData>
@@ -7840,55 +7840,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.198911195717868</v>
+        <v>4.198911196109217</v>
       </c>
       <c r="D2">
-        <v>4.198911195717984</v>
+        <v>4.198911195412807</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>266.6666760066149</v>
+        <v>266.6666760314689</v>
       </c>
       <c r="G2">
-        <v>266.6666760066223</v>
+        <v>266.6666759872409</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.5773502692007634</v>
+        <v>0.5773502691952341</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691799056</v>
+        <v>0.5773502691743765</v>
       </c>
       <c r="Q2">
-        <v>-3.255080704450846E-10</v>
+        <v>-5.812881439986264E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999991205</v>
+        <v>179.9999999936331</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7932,22 +7932,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.5773502690917844</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.5773502692819928</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>5.928731505928823E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999993227</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7991,22 +7991,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.5773502690912249</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>6.074334103495646E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.9999999966301</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -8050,22 +8050,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.5773502690910381</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>7.901494558669101E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999957326</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -8109,22 +8109,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5773502690910381</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>7.901496713604175E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999957326</v>
       </c>
     </row>
   </sheetData>
@@ -8358,55 +8358,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.198911195717868</v>
+        <v>4.198911196109217</v>
       </c>
       <c r="D2">
-        <v>4.198911195717984</v>
+        <v>4.198911195412807</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>266.6666760066149</v>
+        <v>266.6666760314689</v>
       </c>
       <c r="G2">
-        <v>266.6666760066223</v>
+        <v>266.6666759872409</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.5773502692007634</v>
+        <v>0.5773502691952341</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691799056</v>
+        <v>0.5773502691743765</v>
       </c>
       <c r="Q2">
-        <v>-3.255080704450846E-10</v>
+        <v>-5.812881439986264E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999991205</v>
+        <v>179.9999999936331</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -8450,22 +8450,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.5773502690917844</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.5773502692819928</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>5.928731505928823E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999993227</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -8509,22 +8509,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.5773502690912249</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>6.074334103495646E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.9999999966301</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -8568,22 +8568,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.5773502690910381</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>7.901494558669101E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999957326</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -8627,22 +8627,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5773502690910381</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>7.901496713604175E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999957326</v>
       </c>
     </row>
   </sheetData>
@@ -8725,55 +8725,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138798344</v>
+        <v>3.012913138951923</v>
       </c>
       <c r="D2">
-        <v>3.012913138798392</v>
+        <v>3.012913138593917</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.3456832903202</v>
+        <v>191.3456833000739</v>
       </c>
       <c r="G2">
-        <v>191.3456832903233</v>
+        <v>191.3456832773374</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.7472997527179239</v>
+        <v>0.7472997527192564</v>
       </c>
       <c r="O2">
-        <v>0.3354590831704711</v>
+        <v>0.3354590831689602</v>
       </c>
       <c r="P2">
-        <v>0.6184267550144409</v>
+        <v>0.6184267550384416</v>
       </c>
       <c r="Q2">
-        <v>8.10915832045764</v>
+        <v>8.109158318802299</v>
       </c>
       <c r="R2">
-        <v>-117.0248837790425</v>
+        <v>-117.0248837767961</v>
       </c>
       <c r="S2">
-        <v>161.7746336336087</v>
+        <v>161.7746336318227</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -8817,22 +8817,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.7472997526418617</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.335459083077057</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.6184267550841057</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>8.109158321931416</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837562165</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>161.7746336387373</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -8876,22 +8876,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.7472997526385895</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.3354590831006831</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.6184267551237347</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>8.109158324959909</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837452073</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>161.7746336388059</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -8935,22 +8935,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.3354590831085585</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>8.109158325969418</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837415376</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>161.7746336388288</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -8994,22 +8994,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.3354590831085585</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>8.109158325969414</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837415376</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>161.7746336388288</v>
       </c>
     </row>
   </sheetData>
@@ -9092,55 +9092,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138798344</v>
+        <v>3.012913138951923</v>
       </c>
       <c r="D2">
-        <v>3.012913138798392</v>
+        <v>3.012913138593917</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.3456832903202</v>
+        <v>191.3456833000739</v>
       </c>
       <c r="G2">
-        <v>191.3456832903233</v>
+        <v>191.3456832773374</v>
       </c>
       <c r="H2">
-        <v>1.504993719879962</v>
+        <v>1.504993724976225</v>
       </c>
       <c r="I2">
-        <v>15.04993697245902</v>
+        <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993720430847</v>
+        <v>1.504993721246248</v>
       </c>
       <c r="K2">
-        <v>15.04993697341311</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.504993719879901</v>
+        <v>1.504993720695295</v>
       </c>
       <c r="M2">
-        <v>15.04993697245807</v>
+        <v>15.04993697229335</v>
       </c>
       <c r="N2">
-        <v>0.7472997527179239</v>
+        <v>0.7472997527192564</v>
       </c>
       <c r="O2">
-        <v>0.3354590831704711</v>
+        <v>0.3354590831689602</v>
       </c>
       <c r="P2">
-        <v>0.6184267550144409</v>
+        <v>0.6184267550384416</v>
       </c>
       <c r="Q2">
-        <v>8.10915832045764</v>
+        <v>8.109158318802299</v>
       </c>
       <c r="R2">
-        <v>-117.0248837790425</v>
+        <v>-117.0248837767961</v>
       </c>
       <c r="S2">
-        <v>161.7746336336087</v>
+        <v>161.7746336318227</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -9184,22 +9184,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.7472997526418617</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.335459083077057</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.6184267550841057</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999878</v>
+        <v>8.109158321931416</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837562165</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>161.7746336387373</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -9243,22 +9243,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.7472997526385895</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.3354590831006831</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.6184267551237347</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999878</v>
+        <v>8.109158324959909</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837452073</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>161.7746336388059</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -9302,22 +9302,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0.3354590831085585</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999878</v>
+        <v>8.109158325969418</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837415376</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>161.7746336388288</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -9361,22 +9361,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.3354590831085585</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999878</v>
+        <v>8.109158325969414</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>-117.0248837415376</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>161.7746336388288</v>
       </c>
     </row>
   </sheetData>
@@ -10214,49 +10214,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.54545480308452</v>
+        <v>4.545454803106412</v>
       </c>
       <c r="D2">
-        <v>4.54545480308452</v>
+        <v>4.545454803106412</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>288.6751509565138</v>
+        <v>288.6751509579041</v>
       </c>
       <c r="G2">
-        <v>288.6751509565138</v>
+        <v>288.6751509579041</v>
       </c>
       <c r="H2">
-        <v>1.324394473472839</v>
+        <v>1.324394477419387</v>
       </c>
       <c r="I2">
-        <v>13.24394453576828</v>
+        <v>13.24394453497101</v>
       </c>
       <c r="J2">
-        <v>1.324394473554608</v>
+        <v>1.324394474186051</v>
       </c>
       <c r="K2">
-        <v>13.24394453590985</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394473472784</v>
+        <v>1.324394474104236</v>
       </c>
       <c r="M2">
-        <v>13.24394453576745</v>
+        <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.9526279647803683</v>
+        <v>0.9526279647803685</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.9526279647833883</v>
+        <v>0.9526279647833882</v>
       </c>
       <c r="Q2">
-        <v>-8.693883187637584E-11</v>
+        <v>-8.693997994959665E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -10306,22 +10306,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.100000023841858</v>
+        <v>0.952627964667196</v>
       </c>
       <c r="O3">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1.100000023841858</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>29.99999999999879</v>
+        <v>1.45740960157308E-10</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>149.9999999999939</v>
+        <v>179.9999999998456</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -10365,22 +10365,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.100000023841858</v>
+        <v>0.9526279646404244</v>
       </c>
       <c r="O4">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1.100000023841858</v>
+        <v>0.9526279649233318</v>
       </c>
       <c r="Q4">
-        <v>29.99999999999879</v>
+        <v>1.564854331620535E-09</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>149.9999999999939</v>
+        <v>179.9999999984264</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -10424,22 +10424,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.100000023841858</v>
+        <v>0.9526279646315008</v>
       </c>
       <c r="O5">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>1.100000023841858</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q5">
-        <v>29.99999999999879</v>
+        <v>2.037891952334428E-09</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>149.9999999999939</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -10483,22 +10483,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.100000023841858</v>
+        <v>0.9526279646315009</v>
       </c>
       <c r="O6">
-        <v>1.100000023841858</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1.100000023841858</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q6">
-        <v>29.99999999999879</v>
+        <v>2.037888002295718E-09</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999635</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>149.9999999999939</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>